<commit_message>
mise a jour de la doc
</commit_message>
<xml_diff>
--- a/Planification-Initial-SpicyNvaders-theorlando.xlsx
+++ b/Planification-Initial-SpicyNvaders-theorlando.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Theo\Documents\GitHub\Spicy-Nvader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theorlando\Documents\GitHub\Spicy-Nvader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8112E2A7-ABA6-4815-B318-4ECA82C5491D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E38D456-B020-4D2B-9381-8D08CFF57E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16005" yWindow="2670" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -397,7 +394,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>